<commit_message>
adding feedback to the analysis
</commit_message>
<xml_diff>
--- a/gui/mat_mech_linearElastic.xlsx
+++ b/gui/mat_mech_linearElastic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danil\repo\porousLab\gui\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F880AA56-F0FC-427B-BBEB-4E23D35441B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC428AED-A851-4131-B2FE-EF375AA5201C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1464" yWindow="1464" windowWidth="17280" windowHeight="8880" xr2:uid="{E77D3B86-60E5-4C01-95BB-1EDAB849D61B}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8880" xr2:uid="{E77D3B86-60E5-4C01-95BB-1EDAB849D61B}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Young modulus</t>
   </si>
@@ -45,6 +45,12 @@
   </si>
   <si>
     <t>Poisson ratio</t>
+  </si>
+  <si>
+    <t>Density</t>
+  </si>
+  <si>
+    <t>kg/m3</t>
   </si>
 </sst>
 </file>
@@ -417,9 +423,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A706208F-70D6-4D11-AA40-F13D46717FE5}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -445,6 +453,17 @@
         <v>0.2</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>2000</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>